<commit_message>
update for the research
</commit_message>
<xml_diff>
--- a/28省市人口政策数据/1-各城市-分表/广州.xlsx
+++ b/28省市人口政策数据/1-各城市-分表/广州.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" state="visible" r:id="rId2"/>
@@ -3008,10 +3008,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.9438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="87.7448979591837"/>
-    <col collapsed="false" hidden="false" max="256" min="3" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.6734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="86.6632653061225"/>
+    <col collapsed="false" hidden="false" max="256" min="3" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3249,21 +3249,21 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="40.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="38.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="38.2040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="35.3673469387755"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="34.9642857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="39.5510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="71.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="7" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="40.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="37.6632653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="34.9642857142857"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="34.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="39.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="71.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="7" width="9.71938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3478,15 +3478,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="10" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="40.5"/>
-    <col collapsed="false" hidden="false" max="256" min="19" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="16" min="10" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="256" min="19" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3732,19 +3732,19 @@
   </sheetPr>
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="47.7857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.4081632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.1785714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="44.1428571428571"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="47.1122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.8673469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.6377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="43.6020408163265"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3958,11 +3958,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="67" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="67" width="70.0612244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="67" width="84.6377551020408"/>
-    <col collapsed="false" hidden="false" max="256" min="4" style="67" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="68" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="67" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="67" width="69.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="67" width="83.5612244897959"/>
+    <col collapsed="false" hidden="false" max="256" min="4" style="67" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="68" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4072,16 +4072,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="33.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.7959183673469"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="52.5102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="256" min="9" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="51.969387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="256" min="9" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4403,10 +4403,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="56.0204081632653"/>
-    <col collapsed="false" hidden="false" max="256" min="3" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="55.3469387755102"/>
+    <col collapsed="false" hidden="false" max="256" min="3" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>